<commit_message>
alle analyse vakked gemerged
</commit_message>
<xml_diff>
--- a/data/raw/INFANL1-2020-2021 EXAM second chance.xlsx
+++ b/data/raw/INFANL1-2020-2021 EXAM second chance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrejdobrkovic/extra/courses/2223datascience/(X3) black/(02) ANL sources/anonymized/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JiaQiang\Desktop\Project DS Analysis\DsAnalysisProject\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB374F9-6388-8642-BF88-36C61C863162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C23A0E-39E1-4C47-A094-2114AC9B7BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="860" windowWidth="27640" windowHeight="15820" xr2:uid="{C311D21E-D206-824C-BC00-185452538089}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C311D21E-D206-824C-BC00-185452538089}"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4862" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4862" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>Expected:</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -1338,22 +1341,22 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="2.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="1"/>
+    <col min="2" max="2" width="2.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="23" width="8.83203125" style="1"/>
-    <col min="24" max="24" width="2.6640625" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.83203125" style="1"/>
+    <col min="4" max="23" width="8.875" style="1"/>
+    <col min="24" max="24" width="2.625" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:24" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1378,7 +1381,7 @@
       <c r="W2" s="3"/>
       <c r="X2" s="4"/>
     </row>
-    <row r="3" spans="2:24" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
       <c r="F3" s="6" t="s">
         <v>24</v>
@@ -1407,11 +1410,11 @@
       </c>
       <c r="X3" s="11"/>
     </row>
-    <row r="4" spans="2:24" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5"/>
       <c r="X4" s="11"/>
     </row>
-    <row r="5" spans="2:24" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="12" t="s">
         <v>16</v>
@@ -1478,7 +1481,7 @@
       </c>
       <c r="X5" s="11"/>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="15" t="s">
         <v>27</v>
@@ -1565,7 +1568,7 @@
       </c>
       <c r="X6" s="11"/>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="15" t="s">
         <v>28</v>
@@ -1652,7 +1655,7 @@
       </c>
       <c r="X7" s="11"/>
     </row>
-    <row r="8" spans="2:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="18" t="s">
         <v>29</v>
@@ -1739,11 +1742,11 @@
       </c>
       <c r="X8" s="11"/>
     </row>
-    <row r="9" spans="2:24" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="X9" s="11"/>
     </row>
-    <row r="10" spans="2:24" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="12" t="s">
         <v>16</v>
@@ -1810,7 +1813,7 @@
       </c>
       <c r="X10" s="11"/>
     </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="15" t="s">
         <v>27</v>
@@ -1897,7 +1900,7 @@
       </c>
       <c r="X11" s="11"/>
     </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="15" t="s">
         <v>28</v>
@@ -1984,7 +1987,7 @@
       </c>
       <c r="X12" s="11"/>
     </row>
-    <row r="13" spans="2:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="5"/>
       <c r="C13" s="18" t="s">
         <v>29</v>
@@ -2071,15 +2074,15 @@
       </c>
       <c r="X13" s="11"/>
     </row>
-    <row r="14" spans="2:24" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="X14" s="11"/>
     </row>
-    <row r="15" spans="2:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="X15" s="11"/>
     </row>
-    <row r="16" spans="2:24" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="5"/>
       <c r="J16" s="6" t="s">
         <v>30</v>
@@ -2101,7 +2104,7 @@
       </c>
       <c r="X16" s="11"/>
     </row>
-    <row r="17" spans="2:24" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="22"/>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
@@ -2126,7 +2129,7 @@
       <c r="W17" s="23"/>
       <c r="X17" s="24"/>
     </row>
-    <row r="18" spans="2:24" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="2:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2138,18 +2141,18 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AT115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="43" width="4.1640625" customWidth="1"/>
+    <col min="4" max="43" width="4.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2287,7 +2290,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2484150</v>
       </c>
@@ -2424,7 +2427,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2473190</v>
       </c>
@@ -2561,7 +2564,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2460524</v>
       </c>
@@ -2698,7 +2701,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2461323</v>
       </c>
@@ -2835,7 +2838,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2478047</v>
       </c>
@@ -2972,7 +2975,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2460514</v>
       </c>
@@ -3109,7 +3112,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2471988</v>
       </c>
@@ -3246,7 +3249,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2465220</v>
       </c>
@@ -3383,7 +3386,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2472746</v>
       </c>
@@ -3520,7 +3523,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2446346</v>
       </c>
@@ -3657,7 +3660,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2460367</v>
       </c>
@@ -3794,7 +3797,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2449007</v>
       </c>
@@ -3931,7 +3934,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2468597</v>
       </c>
@@ -4068,7 +4071,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2462249</v>
       </c>
@@ -4205,7 +4208,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2469091</v>
       </c>
@@ -4342,7 +4345,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2448525</v>
       </c>
@@ -4479,7 +4482,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2601972</v>
       </c>
@@ -4616,7 +4619,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2461221</v>
       </c>
@@ -4753,7 +4756,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2449234</v>
       </c>
@@ -4890,7 +4893,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2365639</v>
       </c>
@@ -5027,7 +5030,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2473029</v>
       </c>
@@ -5164,7 +5167,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2487380</v>
       </c>
@@ -5301,7 +5304,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2460095</v>
       </c>
@@ -5438,7 +5441,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2472834</v>
       </c>
@@ -5575,7 +5578,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2462740</v>
       </c>
@@ -5712,7 +5715,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2475992</v>
       </c>
@@ -5849,7 +5852,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2482072</v>
       </c>
@@ -5986,7 +5989,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2387697</v>
       </c>
@@ -6123,7 +6126,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2479981</v>
       </c>
@@ -6260,7 +6263,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2461409</v>
       </c>
@@ -6397,7 +6400,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2463162</v>
       </c>
@@ -6534,7 +6537,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2486689</v>
       </c>
@@ -6671,7 +6674,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2462258</v>
       </c>
@@ -6808,7 +6811,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2466897</v>
       </c>
@@ -6945,7 +6948,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2471383</v>
       </c>
@@ -7082,7 +7085,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2466477</v>
       </c>
@@ -7219,7 +7222,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2466569</v>
       </c>
@@ -7356,7 +7359,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2462052</v>
       </c>
@@ -7493,7 +7496,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2462671</v>
       </c>
@@ -7630,7 +7633,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2467558</v>
       </c>
@@ -7767,7 +7770,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2470138</v>
       </c>
@@ -7904,7 +7907,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2419913</v>
       </c>
@@ -8041,7 +8044,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2485380</v>
       </c>
@@ -8178,7 +8181,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2486240</v>
       </c>
@@ -8315,7 +8318,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2461838</v>
       </c>
@@ -8452,7 +8455,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2369028</v>
       </c>
@@ -8589,7 +8592,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2468953</v>
       </c>
@@ -8726,7 +8729,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2486018</v>
       </c>
@@ -8863,7 +8866,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2407419</v>
       </c>
@@ -9000,7 +9003,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2472458</v>
       </c>
@@ -9137,7 +9140,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2488322</v>
       </c>
@@ -9274,7 +9277,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2447571</v>
       </c>
@@ -9411,7 +9414,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2470394</v>
       </c>
@@ -9548,7 +9551,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2464574</v>
       </c>
@@ -9685,7 +9688,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2369630</v>
       </c>
@@ -9822,7 +9825,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2470406</v>
       </c>
@@ -9959,7 +9962,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2375249</v>
       </c>
@@ -10096,7 +10099,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2472609</v>
       </c>
@@ -10233,7 +10236,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2474444</v>
       </c>
@@ -10370,7 +10373,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2473919</v>
       </c>
@@ -10507,7 +10510,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2371373</v>
       </c>
@@ -10644,7 +10647,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2466637</v>
       </c>
@@ -10781,7 +10784,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2475836</v>
       </c>
@@ -10918,7 +10921,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2463394</v>
       </c>
@@ -11055,7 +11058,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2477249</v>
       </c>
@@ -11192,7 +11195,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2442433</v>
       </c>
@@ -11329,7 +11332,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2460816</v>
       </c>
@@ -11466,7 +11469,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2448512</v>
       </c>
@@ -11603,7 +11606,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2462438</v>
       </c>
@@ -11740,7 +11743,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2457637</v>
       </c>
@@ -11877,7 +11880,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="72" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2448317</v>
       </c>
@@ -12014,7 +12017,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2461833</v>
       </c>
@@ -12151,7 +12154,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2488264</v>
       </c>
@@ -12288,7 +12291,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2374905</v>
       </c>
@@ -12425,7 +12428,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2446469</v>
       </c>
@@ -12562,7 +12565,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2398054</v>
       </c>
@@ -12699,7 +12702,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2467025</v>
       </c>
@@ -12836,7 +12839,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2460236</v>
       </c>
@@ -12973,7 +12976,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2461348</v>
       </c>
@@ -13110,7 +13113,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2374797</v>
       </c>
@@ -13247,7 +13250,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2472033</v>
       </c>
@@ -13384,7 +13387,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2479407</v>
       </c>
@@ -13521,7 +13524,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2476102</v>
       </c>
@@ -13658,7 +13661,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2464769</v>
       </c>
@@ -13795,7 +13798,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="86" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2471349</v>
       </c>
@@ -13932,7 +13935,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2461100</v>
       </c>
@@ -14069,7 +14072,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2448118</v>
       </c>
@@ -14206,7 +14209,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="89" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2461288</v>
       </c>
@@ -14343,7 +14346,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2477408</v>
       </c>
@@ -14480,7 +14483,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2468759</v>
       </c>
@@ -14617,7 +14620,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="92" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2391565</v>
       </c>
@@ -14754,7 +14757,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2383406</v>
       </c>
@@ -14891,7 +14894,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2474484</v>
       </c>
@@ -15028,7 +15031,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2474652</v>
       </c>
@@ -15165,7 +15168,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2448095</v>
       </c>
@@ -15302,7 +15305,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="97" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2447854</v>
       </c>
@@ -15439,7 +15442,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2367347</v>
       </c>
@@ -15576,7 +15579,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2575386</v>
       </c>
@@ -15713,7 +15716,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="100" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2477415</v>
       </c>
@@ -15850,7 +15853,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2383071</v>
       </c>
@@ -15987,7 +15990,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2489728</v>
       </c>
@@ -16124,7 +16127,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2464875</v>
       </c>
@@ -16261,7 +16264,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="104" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2397335</v>
       </c>
@@ -16398,7 +16401,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2471046</v>
       </c>
@@ -16535,7 +16538,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="106" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2459364</v>
       </c>
@@ -16672,7 +16675,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2397007</v>
       </c>
@@ -16809,7 +16812,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2461897</v>
       </c>
@@ -16946,7 +16949,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="109" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2448788</v>
       </c>
@@ -17083,7 +17086,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="110" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2460275</v>
       </c>
@@ -17220,7 +17223,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2447003</v>
       </c>
@@ -17357,8 +17360,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="1:46" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="3:46" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:46" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="113" spans="3:46" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C113" s="25" t="s">
         <v>32</v>
       </c>
@@ -17529,7 +17532,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="114" spans="3:46" x14ac:dyDescent="0.2">
+    <row r="114" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C114" s="30" t="s">
         <v>33</v>
       </c>
@@ -17702,7 +17705,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="115" spans="3:46" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:46" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C115" s="35"/>
       <c r="D115" s="36">
         <v>1</v>
@@ -17876,12 +17879,12 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="43" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -18012,7 +18015,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2484150</v>
       </c>
@@ -18140,7 +18143,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2473190</v>
       </c>
@@ -18268,7 +18271,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2460524</v>
       </c>
@@ -18396,7 +18399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2461323</v>
       </c>
@@ -18524,7 +18527,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2478047</v>
       </c>
@@ -18652,7 +18655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2460514</v>
       </c>
@@ -18780,7 +18783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2471988</v>
       </c>
@@ -18908,7 +18911,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2465220</v>
       </c>
@@ -19036,7 +19039,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2472746</v>
       </c>
@@ -19164,7 +19167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2446346</v>
       </c>
@@ -19292,7 +19295,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2460367</v>
       </c>
@@ -19420,7 +19423,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2449007</v>
       </c>
@@ -19548,7 +19551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2468597</v>
       </c>
@@ -19676,7 +19679,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2462249</v>
       </c>
@@ -19804,7 +19807,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2469091</v>
       </c>
@@ -19932,7 +19935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2448525</v>
       </c>
@@ -20060,7 +20063,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2601972</v>
       </c>
@@ -20188,7 +20191,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2461221</v>
       </c>
@@ -20316,7 +20319,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2449234</v>
       </c>
@@ -20444,7 +20447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2365639</v>
       </c>
@@ -20572,7 +20575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2473029</v>
       </c>
@@ -20700,7 +20703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2487380</v>
       </c>
@@ -20828,7 +20831,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2460095</v>
       </c>
@@ -20956,7 +20959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2472834</v>
       </c>
@@ -21084,7 +21087,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2462740</v>
       </c>
@@ -21212,7 +21215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2475992</v>
       </c>
@@ -21340,7 +21343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2482072</v>
       </c>
@@ -21468,7 +21471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2387697</v>
       </c>
@@ -21596,7 +21599,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2479981</v>
       </c>
@@ -21724,7 +21727,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2461409</v>
       </c>
@@ -21852,7 +21855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2463162</v>
       </c>
@@ -21980,7 +21983,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2486689</v>
       </c>
@@ -22108,7 +22111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2462258</v>
       </c>
@@ -22236,7 +22239,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2466897</v>
       </c>
@@ -22364,7 +22367,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2471383</v>
       </c>
@@ -22492,7 +22495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2466477</v>
       </c>
@@ -22620,7 +22623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2466569</v>
       </c>
@@ -22748,7 +22751,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2462052</v>
       </c>
@@ -22876,7 +22879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2462671</v>
       </c>
@@ -23004,7 +23007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2467558</v>
       </c>
@@ -23132,7 +23135,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2470138</v>
       </c>
@@ -23260,7 +23263,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2419913</v>
       </c>
@@ -23388,7 +23391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2485380</v>
       </c>
@@ -23516,7 +23519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2486240</v>
       </c>
@@ -23644,7 +23647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2461838</v>
       </c>
@@ -23772,7 +23775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2369028</v>
       </c>
@@ -23900,7 +23903,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2468953</v>
       </c>
@@ -24028,7 +24031,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2486018</v>
       </c>
@@ -24156,7 +24159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2407419</v>
       </c>
@@ -24284,7 +24287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2472458</v>
       </c>
@@ -24412,7 +24415,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2488322</v>
       </c>
@@ -24540,7 +24543,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2447571</v>
       </c>
@@ -24668,7 +24671,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2470394</v>
       </c>
@@ -24796,7 +24799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2464574</v>
       </c>
@@ -24924,7 +24927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2369630</v>
       </c>
@@ -25052,7 +25055,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2470406</v>
       </c>
@@ -25180,7 +25183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2375249</v>
       </c>
@@ -25308,7 +25311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2472609</v>
       </c>
@@ -25436,7 +25439,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2474444</v>
       </c>
@@ -25564,7 +25567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2473919</v>
       </c>
@@ -25692,7 +25695,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2371373</v>
       </c>
@@ -25820,7 +25823,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2466637</v>
       </c>
@@ -25948,7 +25951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2475836</v>
       </c>
@@ -26076,7 +26079,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2463394</v>
       </c>
@@ -26204,7 +26207,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2477249</v>
       </c>
@@ -26332,7 +26335,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2442433</v>
       </c>
@@ -26460,7 +26463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2460816</v>
       </c>
@@ -26588,7 +26591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2448512</v>
       </c>
@@ -26716,7 +26719,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2462438</v>
       </c>
@@ -26844,7 +26847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2457637</v>
       </c>
@@ -26972,7 +26975,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2448317</v>
       </c>
@@ -27100,7 +27103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2461833</v>
       </c>
@@ -27228,7 +27231,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2488264</v>
       </c>
@@ -27356,7 +27359,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2374905</v>
       </c>
@@ -27484,7 +27487,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2446469</v>
       </c>
@@ -27612,7 +27615,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2398054</v>
       </c>
@@ -27740,7 +27743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2467025</v>
       </c>
@@ -27868,7 +27871,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2460236</v>
       </c>
@@ -27996,7 +27999,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2461348</v>
       </c>
@@ -28124,7 +28127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2374797</v>
       </c>
@@ -28252,7 +28255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2472033</v>
       </c>
@@ -28380,7 +28383,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2479407</v>
       </c>
@@ -28508,7 +28511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2476102</v>
       </c>
@@ -28636,7 +28639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2464769</v>
       </c>
@@ -28764,7 +28767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2471349</v>
       </c>
@@ -28892,7 +28895,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2461100</v>
       </c>
@@ -29020,7 +29023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2448118</v>
       </c>
@@ -29148,7 +29151,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2461288</v>
       </c>
@@ -29276,7 +29279,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2477408</v>
       </c>
@@ -29404,7 +29407,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2468759</v>
       </c>
@@ -29532,7 +29535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2391565</v>
       </c>
@@ -29660,7 +29663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2383406</v>
       </c>
@@ -29788,7 +29791,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2474484</v>
       </c>
@@ -29916,7 +29919,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2474652</v>
       </c>
@@ -30044,7 +30047,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2448095</v>
       </c>
@@ -30172,7 +30175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2447854</v>
       </c>
@@ -30300,7 +30303,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2367347</v>
       </c>
@@ -30428,7 +30431,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2575386</v>
       </c>
@@ -30556,7 +30559,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2477415</v>
       </c>
@@ -30684,7 +30687,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2383071</v>
       </c>
@@ -30812,7 +30815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2489728</v>
       </c>
@@ -30940,7 +30943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2464875</v>
       </c>
@@ -31068,7 +31071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2397335</v>
       </c>
@@ -31196,7 +31199,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2471046</v>
       </c>
@@ -31324,7 +31327,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2459364</v>
       </c>
@@ -31452,7 +31455,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2397007</v>
       </c>
@@ -31580,7 +31583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="108" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2461897</v>
       </c>
@@ -31708,7 +31711,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2448788</v>
       </c>
@@ -31836,7 +31839,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2460275</v>
       </c>
@@ -31964,7 +31967,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2447003</v>
       </c>
@@ -32092,8 +32095,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:43" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="3:43" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="113" spans="3:43" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C113" s="54" t="s">
         <v>16</v>
       </c>
@@ -32218,7 +32221,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="114" spans="3:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C114" s="57" t="s">
         <v>38</v>
       </c>
@@ -32343,7 +32346,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="115" spans="3:43" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="3:43" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C115" s="60" t="s">
         <v>5</v>
       </c>
@@ -32508,7 +32511,7 @@
         <v>0.26363636363636361</v>
       </c>
     </row>
-    <row r="116" spans="3:43" x14ac:dyDescent="0.2">
+    <row r="116" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C116" s="44" t="s">
         <v>4</v>
       </c>
@@ -32673,7 +32676,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="117" spans="3:43" x14ac:dyDescent="0.2">
+    <row r="117" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C117" s="44" t="s">
         <v>6</v>
       </c>
@@ -32838,7 +32841,7 @@
         <v>0.27272727272727271</v>
       </c>
     </row>
-    <row r="118" spans="3:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C118" s="61" t="s">
         <v>7</v>
       </c>
@@ -33003,7 +33006,7 @@
         <v>0.26363636363636361</v>
       </c>
     </row>
-    <row r="119" spans="3:43" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="119" spans="3:43" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33017,13 +33020,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
     <col min="2" max="3" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>35</v>
       </c>
@@ -33043,7 +33046,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
         <v>13</v>
       </c>
@@ -33065,7 +33068,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
         <v>15</v>
       </c>
@@ -33083,7 +33086,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
         <v>5</v>
       </c>
@@ -33101,7 +33104,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>4</v>
       </c>
@@ -33119,7 +33122,7 @@
         <v>0.45454545454545453</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
         <v>6</v>
       </c>
@@ -33137,7 +33140,7 @@
         <v>0.18181818181818182</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
         <v>7</v>
       </c>
@@ -33155,7 +33158,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
         <v>14</v>
       </c>
@@ -33173,7 +33176,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
         <v>3</v>
       </c>
@@ -33191,7 +33194,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>11</v>
       </c>
@@ -33209,7 +33212,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
         <v>10</v>
       </c>
@@ -33227,7 +33230,7 @@
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
         <v>12</v>
       </c>
@@ -33245,7 +33248,7 @@
         <v>0.22222222222222221</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="51" t="s">
         <v>8</v>
       </c>
@@ -33263,7 +33266,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33278,9 +33281,9 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -33288,7 +33291,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -33296,7 +33299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -33304,7 +33307,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -33312,7 +33315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -33320,7 +33323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -33328,7 +33331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -33336,7 +33339,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -33344,7 +33347,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -33352,7 +33355,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -33360,7 +33363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -33368,7 +33371,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -33376,7 +33379,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -33384,7 +33387,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -33392,7 +33395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -33400,7 +33403,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -33408,7 +33411,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -33416,7 +33419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -33424,7 +33427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -33432,7 +33435,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -33440,7 +33443,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -33448,7 +33451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -33456,7 +33459,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -33464,7 +33467,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -33472,7 +33475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -33480,7 +33483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -33488,7 +33491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -33496,7 +33499,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -33504,7 +33507,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -33512,7 +33515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -33520,7 +33523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -33528,7 +33531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -33536,7 +33539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -33544,7 +33547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -33552,7 +33555,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -33560,7 +33563,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -33568,7 +33571,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -33576,7 +33579,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -33584,7 +33587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -33592,7 +33595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -33600,7 +33603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>

</xml_diff>